<commit_message>
import north coast south admin and reflect stream order proxy classification. Added data source to fwa tables. Updated buffer code to use max percentage as Gord requested. Added export to gdb steps (not currently working). Started buffering steps.
</commit_message>
<xml_diff>
--- a/data/analysis/stream_order_proxies_TSA.xlsx
+++ b/data/analysis/stream_order_proxies_TSA.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\THLB_Proxy\data\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FF31B7-C382-45D2-AB68-3F2D5C6EEFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D43893C-1645-4F50-8771-5F6453888B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26140" yWindow="660" windowWidth="12140" windowHeight="19580" xr2:uid="{896D4BF2-6796-401A-A905-2BDC8D3E45E0}"/>
+    <workbookView xWindow="31476" yWindow="300" windowWidth="25284" windowHeight="16164" activeTab="1" xr2:uid="{896D4BF2-6796-401A-A905-2BDC8D3E45E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$U$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="144">
   <si>
     <t>Pacific</t>
   </si>
@@ -359,10 +362,118 @@
     <t>38.5</t>
   </si>
   <si>
-    <t>divided by operating area within bulkley</t>
-  </si>
-  <si>
     <t>tsa_number</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>Table shared by David Stuart, July 25, 2024 "shared from folks at Smithers"</t>
+  </si>
+  <si>
+    <t>Data Package</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/100_mile_house_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/arrowsmith_tsa_data_package_updated.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/arrow_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/boundary_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>broken up by areas</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/cascadia_tsa_draft_information_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/cassiar_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/cranbrook_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/dawson_creek_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>bold = reviewed for reduction/retention</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/fort_st_john_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/08tsdp18_updated.pdf</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/fraser_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>Haida Gwaii</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/invermere_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/kalum_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/kamloops_tsa_data_package.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/12ts_dp_updated_jan_2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/13ts_dpkg_2020_november.pdf</t>
+  </si>
+  <si>
+    <t>14.5</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/14tsdp_update_apr2019.pdf</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/15ts_dpkg_jan2021.pdf</t>
+  </si>
+  <si>
+    <t>Kelly aspatial</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/16ts_dp_2020_november.pdf</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Prince George ****</t>
+  </si>
+  <si>
+    <t>**** stopped reviewing as spoke with Gord and going with Riparian management guidelines</t>
   </si>
 </sst>
 </file>
@@ -762,26 +873,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8A07E1-079B-4967-B95F-C8A23FAFCBF0}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.54296875" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.90625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -808,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -837,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -863,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -889,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -900,7 +1011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -911,7 +1022,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -937,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -963,7 +1074,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -989,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1000,7 +1111,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1011,7 +1122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1022,7 +1133,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1033,7 +1144,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1044,7 +1155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1055,7 +1166,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1066,7 +1177,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1077,7 +1188,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1088,7 +1199,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1099,7 +1210,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1110,7 +1221,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1121,7 +1232,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1132,7 +1243,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1143,7 +1254,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1154,7 +1265,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1165,7 +1276,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1176,7 +1287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1187,7 +1298,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1198,7 +1309,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -1209,7 +1320,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1220,7 +1331,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1231,7 +1342,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1242,7 +1353,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1250,7 +1361,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1276,7 +1387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1292,22 +1403,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A024854-562A-4BA3-B5BC-18078DDE4ADF}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="4" max="20" width="8.7265625" style="8"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="5" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="7.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="5.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -1363,96 +1482,51 @@
       <c r="T1" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
+      <c r="U1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="P2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="E3" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>86</v>
@@ -1463,41 +1537,33 @@
       <c r="L3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="N3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>19</v>
+        <v>81</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>90</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
         <v>91</v>
       </c>
@@ -1516,31 +1582,19 @@
       <c r="J4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T4" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>21</v>
+      <c r="U4" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>90</v>
@@ -1566,10 +1620,10 @@
       <c r="K5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>80</v>
       </c>
       <c r="P5" s="8" t="s">
@@ -1581,544 +1635,698 @@
       <c r="T5" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>24</v>
+      <c r="U5" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="B10">
+        <v>41</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G14" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="8" t="s">
+      <c r="H14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="N10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P10" s="8" t="s">
+      <c r="N14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="R10" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T10" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="R11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="S11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="T11" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12">
-        <v>41</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14">
-        <v>40</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="R14" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="T14" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15">
-        <v>30</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>94</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>89</v>
       </c>
       <c r="M15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N16" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="N15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="P15" s="8" t="s">
+      <c r="O16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q16" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="R16" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="R15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="T15" s="8" t="s">
+      <c r="S16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="E17" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T17" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="R16" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17">
-        <v>9</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N17" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="O17" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="P17" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q17" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="R17" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="S17" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="T17" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>48</v>
+      <c r="U17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>86</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>89</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>80</v>
+        <v>89</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="P18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="D19" s="8">
+        <v>20</v>
+      </c>
+      <c r="E19" s="8">
+        <v>54</v>
+      </c>
+      <c r="F19" s="8">
+        <v>34</v>
+      </c>
+      <c r="G19" s="8">
+        <v>24</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="R18" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T18" s="8" t="s">
+      <c r="R19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T19" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19">
-        <v>11</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J19" s="8" t="s">
+      <c r="E20" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N19" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="R19" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="S19" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T19" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20">
-        <v>12</v>
-      </c>
-      <c r="D20" s="8">
-        <v>20</v>
-      </c>
-      <c r="E20" s="8">
-        <v>54</v>
-      </c>
-      <c r="F20" s="8">
-        <v>34</v>
-      </c>
-      <c r="G20" s="8">
-        <v>24</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="N20" s="8" t="s">
         <v>80</v>
@@ -2132,174 +2340,295 @@
       <c r="T20" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>52</v>
+      <c r="U20" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="R21" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="T21" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="V21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="D22" s="8">
+        <v>35</v>
+      </c>
+      <c r="E22" s="8">
+        <v>57</v>
+      </c>
+      <c r="F22" s="8">
+        <v>35</v>
+      </c>
+      <c r="G22" s="8">
+        <v>25</v>
+      </c>
+      <c r="H22" s="8">
+        <v>8</v>
+      </c>
+      <c r="I22" s="8">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8">
+        <v>3</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0</v>
+      </c>
+      <c r="L22" s="8">
+        <v>10</v>
+      </c>
+      <c r="M22" s="8">
+        <v>15</v>
+      </c>
+      <c r="N22" s="8">
+        <v>7</v>
+      </c>
+      <c r="O22" s="8">
+        <v>7</v>
+      </c>
+      <c r="P22" s="8">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>15</v>
+      </c>
+      <c r="R22" s="8">
+        <v>7</v>
+      </c>
+      <c r="S22" s="8">
+        <v>6</v>
+      </c>
+      <c r="T22" s="8">
+        <v>19</v>
+      </c>
+      <c r="V22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22">
-        <v>14</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23">
-        <v>15</v>
-      </c>
-      <c r="D23" s="8">
-        <v>35</v>
-      </c>
-      <c r="E23" s="8">
-        <v>57</v>
-      </c>
-      <c r="F23" s="8">
-        <v>35</v>
-      </c>
-      <c r="G23" s="8">
-        <v>25</v>
-      </c>
-      <c r="H23" s="8">
-        <v>8</v>
-      </c>
-      <c r="I23" s="8">
-        <v>8</v>
-      </c>
-      <c r="J23" s="8">
-        <v>3</v>
-      </c>
-      <c r="K23" s="8">
-        <v>0</v>
-      </c>
-      <c r="L23" s="8">
-        <v>10</v>
-      </c>
-      <c r="M23" s="8">
-        <v>15</v>
-      </c>
-      <c r="N23" s="8">
-        <v>7</v>
-      </c>
-      <c r="O23" s="8">
-        <v>7</v>
-      </c>
-      <c r="P23" s="8">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>15</v>
-      </c>
-      <c r="R23" s="8">
-        <v>7</v>
-      </c>
-      <c r="S23" s="8">
-        <v>6</v>
-      </c>
-      <c r="T23" s="8">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>55</v>
+      <c r="V23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B24">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>56</v>
+      <c r="U24" s="8"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="P25" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="T25" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="U25" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26">
+        <v>43</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>48</v>
+      </c>
+      <c r="D27" s="8">
+        <v>60</v>
+      </c>
+      <c r="E27" s="8">
+        <v>60</v>
+      </c>
+      <c r="F27" s="8">
+        <v>35</v>
+      </c>
+      <c r="G27" s="8">
+        <v>30</v>
+      </c>
+      <c r="H27" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="I27" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="J27" s="8">
+        <v>1</v>
+      </c>
+      <c r="K27" s="8">
+        <v>10</v>
+      </c>
+      <c r="L27" s="8">
+        <v>10</v>
+      </c>
+      <c r="M27" s="8">
+        <v>15</v>
+      </c>
+      <c r="N27" s="8">
+        <v>15</v>
+      </c>
+      <c r="O27" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="P27" s="8">
         <v>20</v>
       </c>
-      <c r="E26" s="8">
-        <v>60</v>
-      </c>
-      <c r="F26" s="8">
-        <v>40</v>
-      </c>
-      <c r="G26" s="8">
-        <v>30</v>
-      </c>
-      <c r="L26" s="8">
-        <v>10</v>
-      </c>
-      <c r="P26" s="8">
+      <c r="Q27" s="8">
         <v>20</v>
       </c>
-      <c r="T26" s="8">
+      <c r="R27" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="S27" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="T27" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27">
-        <v>43</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>9</v>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B28">
         <v>22</v>
       </c>
       <c r="D28" s="8">
-        <v>60</v>
+        <v>12.4</v>
       </c>
       <c r="E28" s="8">
-        <v>60</v>
+        <v>12.4</v>
       </c>
       <c r="F28" s="8">
-        <v>35</v>
+        <v>12.4</v>
       </c>
       <c r="G28" s="8">
-        <v>30</v>
+        <v>12.4</v>
       </c>
       <c r="H28" s="8">
-        <v>7.5</v>
+        <v>12.4</v>
       </c>
       <c r="I28" s="8">
-        <v>7.5</v>
+        <v>12.4</v>
       </c>
       <c r="J28" s="8">
-        <v>1</v>
+        <v>12.4</v>
       </c>
       <c r="K28" s="8">
         <v>10</v>
@@ -2311,7 +2640,7 @@
         <v>15</v>
       </c>
       <c r="N28" s="8">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="O28" s="8">
         <v>7.5</v>
@@ -2320,7 +2649,7 @@
         <v>20</v>
       </c>
       <c r="Q28" s="8">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="R28" s="8">
         <v>7.5</v>
@@ -2332,36 +2661,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>59</v>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="B29">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D29" s="8">
-        <v>12.4</v>
+        <v>50</v>
       </c>
       <c r="E29" s="8">
-        <v>12.4</v>
+        <v>60</v>
       </c>
       <c r="F29" s="8">
-        <v>12.4</v>
+        <v>40</v>
       </c>
       <c r="G29" s="8">
-        <v>12.4</v>
+        <v>30</v>
       </c>
       <c r="H29" s="8">
-        <v>12.4</v>
+        <v>7.5</v>
       </c>
       <c r="I29" s="8">
-        <v>12.4</v>
+        <v>7.5</v>
       </c>
       <c r="J29" s="8">
-        <v>12.4</v>
+        <v>1</v>
       </c>
       <c r="K29" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L29" s="8">
         <v>10</v>
@@ -2391,117 +2720,102 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>0</v>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B30">
-        <v>26</v>
-      </c>
-      <c r="D30" s="8">
-        <v>50</v>
-      </c>
-      <c r="E30" s="8">
+        <v>27</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31">
+        <v>17</v>
+      </c>
+      <c r="D31" s="8">
+        <v>20</v>
+      </c>
+      <c r="E31" s="8">
         <v>60</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F31" s="8">
         <v>40</v>
       </c>
-      <c r="G30" s="8">
-        <v>30</v>
-      </c>
-      <c r="H30" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="I30" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="J30" s="8">
-        <v>1</v>
-      </c>
-      <c r="K30" s="8">
-        <v>0</v>
-      </c>
-      <c r="L30" s="8">
-        <v>10</v>
-      </c>
-      <c r="M30" s="8">
-        <v>15</v>
-      </c>
-      <c r="N30" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="O30" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="P30" s="8">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="8">
-        <v>15</v>
-      </c>
-      <c r="R30" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="S30" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="T30" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31">
-        <v>27</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D32" s="8">
         <v>20</v>
       </c>
       <c r="E32" s="8">
+        <v>54</v>
+      </c>
+      <c r="F32" s="8">
+        <v>34</v>
+      </c>
+      <c r="G32" s="8">
+        <v>24</v>
+      </c>
+      <c r="H32" s="8">
+        <v>3</v>
+      </c>
+      <c r="I32" s="8">
+        <v>3</v>
+      </c>
+      <c r="J32" s="8">
+        <v>0</v>
+      </c>
+      <c r="K32" s="8">
+        <v>10</v>
+      </c>
+      <c r="N32" s="8">
+        <v>3</v>
+      </c>
+      <c r="P32" s="8">
+        <v>14</v>
+      </c>
+      <c r="R32" s="8">
+        <v>3</v>
+      </c>
+      <c r="T32" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33">
+        <v>39</v>
+      </c>
+      <c r="D33" s="8">
         <v>60</v>
       </c>
-      <c r="F32" s="8">
+      <c r="E33" s="8">
+        <v>60</v>
+      </c>
+      <c r="F33" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33">
-        <v>31</v>
-      </c>
-      <c r="D33" s="8">
+      <c r="G33" s="8">
         <v>20</v>
       </c>
-      <c r="E33" s="8">
-        <v>54</v>
-      </c>
-      <c r="F33" s="8">
-        <v>34</v>
-      </c>
-      <c r="G33" s="8">
-        <v>24</v>
-      </c>
       <c r="H33" s="8">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I33" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J33" s="8">
         <v>0</v>
@@ -2510,27 +2824,27 @@
         <v>10</v>
       </c>
       <c r="N33" s="8">
-        <v>3</v>
+        <v>7.5</v>
       </c>
       <c r="P33" s="8">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="R33" s="8">
-        <v>3</v>
+        <v>7.5</v>
       </c>
       <c r="T33" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B34">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D34" s="8">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E34" s="8">
         <v>60</v>
@@ -2539,90 +2853,108 @@
         <v>40</v>
       </c>
       <c r="G34" s="8">
+        <v>30</v>
+      </c>
+      <c r="H34" s="8">
+        <v>15</v>
+      </c>
+      <c r="I34" s="8">
+        <v>15</v>
+      </c>
+      <c r="J34" s="8">
+        <v>10</v>
+      </c>
+      <c r="L34" s="8">
+        <v>10</v>
+      </c>
+      <c r="M34" s="8">
         <v>20</v>
       </c>
-      <c r="H34" s="8">
+      <c r="N34" s="8">
+        <v>15</v>
+      </c>
+      <c r="O34" s="8">
+        <v>15</v>
+      </c>
+      <c r="P34" s="8">
+        <v>30</v>
+      </c>
+      <c r="Q34" s="8">
         <v>20</v>
       </c>
-      <c r="I34" s="8">
-        <v>0</v>
-      </c>
-      <c r="J34" s="8">
-        <v>0</v>
-      </c>
-      <c r="K34" s="8">
-        <v>10</v>
-      </c>
-      <c r="N34" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="P34" s="8">
+      <c r="R34" s="8">
+        <v>15</v>
+      </c>
+      <c r="S34" s="8">
+        <v>15</v>
+      </c>
+      <c r="T34" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="R34" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="T34" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35">
-        <v>29</v>
-      </c>
-      <c r="D35" s="8">
-        <v>50</v>
-      </c>
-      <c r="E35" s="8">
-        <v>60</v>
-      </c>
-      <c r="F35" s="8">
-        <v>40</v>
-      </c>
-      <c r="G35" s="8">
-        <v>30</v>
-      </c>
-      <c r="H35" s="8">
-        <v>15</v>
-      </c>
-      <c r="I35" s="8">
-        <v>15</v>
-      </c>
-      <c r="J35" s="8">
-        <v>10</v>
-      </c>
-      <c r="L35" s="8">
-        <v>10</v>
-      </c>
-      <c r="M35" s="8">
-        <v>20</v>
-      </c>
-      <c r="N35" s="8">
-        <v>15</v>
-      </c>
-      <c r="O35" s="8">
-        <v>15</v>
-      </c>
-      <c r="P35" s="8">
-        <v>30</v>
-      </c>
-      <c r="Q35" s="8">
-        <v>20</v>
-      </c>
-      <c r="R35" s="8">
-        <v>15</v>
-      </c>
-      <c r="S35" s="8">
-        <v>15</v>
-      </c>
-      <c r="T35" s="8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D35" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q35" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="R35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S35" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T35" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2678,7 +3010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -2728,7 +3060,23 @@
         <v>20</v>
       </c>
     </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:U37" xr:uid="{2A024854-562A-4BA3-B5BC-18078DDE4ADF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U37">
+      <sortCondition ref="A1:A37"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Altered linear_weight to take in more arguments and moved into functions scripts
</commit_message>
<xml_diff>
--- a/data/analysis/stream_order_proxies_TSA.xlsx
+++ b/data/analysis/stream_order_proxies_TSA.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\THLB_Proxy\data\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D43893C-1645-4F50-8771-5F6453888B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9C2F66-053A-49EC-9968-999245A4DFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31476" yWindow="300" windowWidth="25284" windowHeight="16164" activeTab="1" xr2:uid="{896D4BF2-6796-401A-A905-2BDC8D3E45E0}"/>
+    <workbookView xWindow="330" yWindow="300" windowWidth="26940" windowHeight="19320" activeTab="1" xr2:uid="{896D4BF2-6796-401A-A905-2BDC8D3E45E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$U$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$U$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="150">
   <si>
     <t>Pacific</t>
   </si>
@@ -474,13 +474,32 @@
   </si>
   <si>
     <t>**** stopped reviewing as spoke with Gord and going with Riparian management guidelines</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>A comprehensive riparian classification inventory is not available for the TSA. The permanent riparian reserve aspatial netdown from the previous two reviews will be carried
+forward for the current analysis</t>
+  </si>
+  <si>
+    <t>Riparian Management Guidebook</t>
+  </si>
+  <si>
+    <t>Section 52, FRPA</t>
+  </si>
+  <si>
+    <t>https://www2.gov.bc.ca/assets/gov/farming-natural-resources-and-industry/forestry/stewardship/forest-analysis-inventory/tsr-annual-allowable-cut/okanagan_tsa_datapackage_2017.pdf</t>
+  </si>
+  <si>
+    <t>At this time there is not a data base that identifies a stream class for each stream reach within the Okanagan TSA. Instead of a specific riparian buffer for each stream class, a weighted average riparian buffer width across all streams, that was calculated for the Okanagan TSA based on an assessment of stream class distribution by Wild Stone Resources, will be used. This average reserve width of 12.4 metres is applied to each side of all streams (S1 to S6) identified in the Okanagan TSA timber supply review file (FWA-based streams).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,13 +515,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -514,10 +545,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,8 +569,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1403,16 +1441,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A024854-562A-4BA3-B5BC-18078DDE4ADF}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" customWidth="1"/>
     <col min="4" max="5" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -1422,9 +1460,10 @@
     <col min="15" max="15" width="5.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="20" width="5.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.109375" customWidth="1"/>
+    <col min="23" max="23" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>106</v>
       </c>
@@ -1488,113 +1527,162 @@
       <c r="V1" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W1" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="9" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B2">
+      <c r="B4" s="9">
         <v>23</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V4" s="9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="W4" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
+      <c r="B5">
         <v>1</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="V3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4">
-        <v>38</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="V4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>90</v>
@@ -1620,10 +1708,10 @@
       <c r="K5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>80</v>
       </c>
       <c r="P5" s="8" t="s">
@@ -1639,643 +1727,611 @@
         <v>112</v>
       </c>
       <c r="V5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="F7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="R6" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="U6" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>118</v>
+      <c r="O7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="U7" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>91</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>89</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="U8" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="V8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="S9" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>118</v>
       </c>
       <c r="U9" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B10">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>83</v>
+        <v>93</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="U10" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>46</v>
+        <v>95</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="U11" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="L12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="R12" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="T12" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U12" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q13" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="R13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="S13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="T13" s="8" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="U13" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="L14" s="8" t="s">
+      <c r="N14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>89</v>
       </c>
       <c r="M15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="U15" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="N15" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q15" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16">
-        <v>9</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q16" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="R16" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="S16" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="T16" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="U16" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="V16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>86</v>
+        <v>128</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>89</v>
       </c>
       <c r="M17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="O17" s="8" t="s">
         <v>80</v>
       </c>
       <c r="P17" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q17" s="8" t="s">
         <v>81</v>
       </c>
       <c r="R17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="S17" s="8" t="s">
         <v>80</v>
       </c>
       <c r="T17" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="M18" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="U17" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="V17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18">
-        <v>11</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="N18" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P18" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="R18" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="Q18" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="R18" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="S18" s="8" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="U18" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19">
-        <v>12</v>
-      </c>
-      <c r="D19" s="8">
-        <v>20</v>
-      </c>
-      <c r="E19" s="8">
-        <v>54</v>
-      </c>
-      <c r="F19" s="8">
-        <v>34</v>
-      </c>
-      <c r="G19" s="8">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="N19" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M19" s="8" t="s">
         <v>80</v>
       </c>
       <c r="P19" s="8" t="s">
@@ -2285,397 +2341,397 @@
         <v>80</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="U19" s="8" t="s">
         <v>112</v>
       </c>
       <c r="V19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="9">
+        <v>11</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="U20" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="V20" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="D21" s="8">
+        <v>20</v>
+      </c>
+      <c r="E21" s="8">
+        <v>54</v>
+      </c>
+      <c r="F21" s="8">
+        <v>34</v>
+      </c>
+      <c r="G21" s="8">
+        <v>24</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="R21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T21" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="U21" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="V21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>13</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J20" s="8" t="s">
+      <c r="H22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K22" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L22" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="N20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="P20" s="8" t="s">
+      <c r="N22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="R20" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T20" s="8" t="s">
+      <c r="R22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="U20" s="8" t="s">
+      <c r="U22" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="V20" t="s">
+      <c r="V22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>14</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G23" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H23" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I23" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="L21" s="8" t="s">
+      <c r="L23" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="N21" s="8" t="s">
+      <c r="N23" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="P23" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="R21" s="8" t="s">
+      <c r="R23" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="T21" s="8" t="s">
+      <c r="T23" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="V21" t="s">
+      <c r="V23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>15</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D24" s="8">
         <v>35</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E24" s="8">
         <v>57</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F24" s="8">
         <v>35</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G24" s="8">
         <v>25</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H24" s="8">
         <v>8</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I24" s="8">
         <v>8</v>
       </c>
-      <c r="J22" s="8">
+      <c r="J24" s="8">
         <v>3</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K24" s="8">
         <v>0</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L24" s="8">
         <v>10</v>
       </c>
-      <c r="M22" s="8">
+      <c r="M24" s="8">
         <v>15</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N24" s="8">
         <v>7</v>
       </c>
-      <c r="O22" s="8">
+      <c r="O24" s="8">
         <v>7</v>
       </c>
-      <c r="P22" s="8">
+      <c r="P24" s="8">
         <v>19</v>
       </c>
-      <c r="Q22" s="8">
+      <c r="Q24" s="8">
         <v>15</v>
       </c>
-      <c r="R22" s="8">
+      <c r="R24" s="8">
         <v>7</v>
       </c>
-      <c r="S22" s="8">
+      <c r="S24" s="8">
         <v>6</v>
       </c>
-      <c r="T22" s="8">
+      <c r="T24" s="8">
         <v>19</v>
       </c>
-      <c r="V22" t="s">
+      <c r="V24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>16</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="V23" t="s">
+      <c r="V25" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B24">
+      <c r="B26">
         <v>18</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="U24" s="8"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25">
-        <v>20</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="P25" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="R25" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="T25" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="U25" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26">
-        <v>43</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="U26" s="8"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="T27" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="U27" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28">
+        <v>43</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>48</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D29" s="8">
         <v>60</v>
-      </c>
-      <c r="E27" s="8">
-        <v>60</v>
-      </c>
-      <c r="F27" s="8">
-        <v>35</v>
-      </c>
-      <c r="G27" s="8">
-        <v>30</v>
-      </c>
-      <c r="H27" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="I27" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="J27" s="8">
-        <v>1</v>
-      </c>
-      <c r="K27" s="8">
-        <v>10</v>
-      </c>
-      <c r="L27" s="8">
-        <v>10</v>
-      </c>
-      <c r="M27" s="8">
-        <v>15</v>
-      </c>
-      <c r="N27" s="8">
-        <v>15</v>
-      </c>
-      <c r="O27" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="P27" s="8">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="8">
-        <v>20</v>
-      </c>
-      <c r="R27" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="S27" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="T27" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28">
-        <v>22</v>
-      </c>
-      <c r="D28" s="8">
-        <v>12.4</v>
-      </c>
-      <c r="E28" s="8">
-        <v>12.4</v>
-      </c>
-      <c r="F28" s="8">
-        <v>12.4</v>
-      </c>
-      <c r="G28" s="8">
-        <v>12.4</v>
-      </c>
-      <c r="H28" s="8">
-        <v>12.4</v>
-      </c>
-      <c r="I28" s="8">
-        <v>12.4</v>
-      </c>
-      <c r="J28" s="8">
-        <v>12.4</v>
-      </c>
-      <c r="K28" s="8">
-        <v>10</v>
-      </c>
-      <c r="L28" s="8">
-        <v>10</v>
-      </c>
-      <c r="M28" s="8">
-        <v>15</v>
-      </c>
-      <c r="N28" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="O28" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="P28" s="8">
-        <v>20</v>
-      </c>
-      <c r="Q28" s="8">
-        <v>15</v>
-      </c>
-      <c r="R28" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="S28" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="T28" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29">
-        <v>26</v>
-      </c>
-      <c r="D29" s="8">
-        <v>50</v>
       </c>
       <c r="E29" s="8">
         <v>60</v>
       </c>
       <c r="F29" s="8">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G29" s="8">
         <v>30</v>
@@ -2690,7 +2746,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L29" s="8">
         <v>10</v>
@@ -2699,7 +2755,7 @@
         <v>15</v>
       </c>
       <c r="N29" s="8">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="O29" s="8">
         <v>7.5</v>
@@ -2708,7 +2764,7 @@
         <v>20</v>
       </c>
       <c r="Q29" s="8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="R29" s="8">
         <v>7.5</v>
@@ -2720,26 +2776,80 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B30">
-        <v>27</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>61</v>
+    <row r="30" spans="1:23" s="9" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="9">
+        <v>22</v>
+      </c>
+      <c r="D30" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="E30" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="F30" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="G30" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="H30" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="I30" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="J30" s="11">
+        <v>12.4</v>
+      </c>
+      <c r="K30" s="11">
+        <v>10</v>
+      </c>
+      <c r="L30" s="11">
+        <v>10</v>
+      </c>
+      <c r="M30" s="11">
+        <v>15</v>
+      </c>
+      <c r="N30" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="O30" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="P30" s="11">
+        <v>20</v>
+      </c>
+      <c r="Q30" s="11">
+        <v>15</v>
+      </c>
+      <c r="R30" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="S30" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="T30" s="11">
+        <v>20</v>
+      </c>
+      <c r="V30" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="W30" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D31" s="8">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E31" s="8">
         <v>60</v>
@@ -2747,60 +2857,69 @@
       <c r="F31" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>62</v>
+      <c r="G31" s="8">
+        <v>30</v>
+      </c>
+      <c r="H31" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="I31" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="J31" s="8">
+        <v>1</v>
+      </c>
+      <c r="K31" s="8">
+        <v>0</v>
+      </c>
+      <c r="L31" s="8">
+        <v>10</v>
+      </c>
+      <c r="M31" s="8">
+        <v>15</v>
+      </c>
+      <c r="N31" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="O31" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="P31" s="8">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>15</v>
+      </c>
+      <c r="R31" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="S31" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="T31" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B32">
-        <v>31</v>
-      </c>
-      <c r="D32" s="8">
-        <v>20</v>
-      </c>
-      <c r="E32" s="8">
-        <v>54</v>
-      </c>
-      <c r="F32" s="8">
-        <v>34</v>
-      </c>
-      <c r="G32" s="8">
-        <v>24</v>
-      </c>
-      <c r="H32" s="8">
-        <v>3</v>
-      </c>
-      <c r="I32" s="8">
-        <v>3</v>
-      </c>
-      <c r="J32" s="8">
-        <v>0</v>
-      </c>
-      <c r="K32" s="8">
-        <v>10</v>
-      </c>
-      <c r="N32" s="8">
-        <v>3</v>
-      </c>
-      <c r="P32" s="8">
-        <v>14</v>
-      </c>
-      <c r="R32" s="8">
-        <v>3</v>
-      </c>
-      <c r="T32" s="8">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B33">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D33" s="8">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="E33" s="8">
         <v>60</v>
@@ -2808,155 +2927,101 @@
       <c r="F33" s="8">
         <v>40</v>
       </c>
-      <c r="G33" s="8">
-        <v>20</v>
-      </c>
-      <c r="H33" s="8">
-        <v>20</v>
-      </c>
-      <c r="I33" s="8">
-        <v>0</v>
-      </c>
-      <c r="J33" s="8">
-        <v>0</v>
-      </c>
-      <c r="K33" s="8">
-        <v>10</v>
-      </c>
-      <c r="N33" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="P33" s="8">
-        <v>20</v>
-      </c>
-      <c r="R33" s="8">
-        <v>7.5</v>
-      </c>
-      <c r="T33" s="8">
-        <v>20</v>
-      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B34">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D34" s="8">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E34" s="8">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F34" s="8">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G34" s="8">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H34" s="8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I34" s="8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="J34" s="8">
+        <v>0</v>
+      </c>
+      <c r="K34" s="8">
         <v>10</v>
       </c>
-      <c r="L34" s="8">
-        <v>10</v>
-      </c>
-      <c r="M34" s="8">
-        <v>20</v>
-      </c>
       <c r="N34" s="8">
-        <v>15</v>
-      </c>
-      <c r="O34" s="8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="P34" s="8">
-        <v>30</v>
-      </c>
-      <c r="Q34" s="8">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="R34" s="8">
-        <v>15</v>
-      </c>
-      <c r="S34" s="8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="T34" s="8">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="B35">
         <v>39</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" s="8">
+        <v>60</v>
+      </c>
+      <c r="E35" s="8">
+        <v>60</v>
+      </c>
+      <c r="F35" s="8">
+        <v>40</v>
+      </c>
+      <c r="G35" s="8">
         <v>20</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="O35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="P35" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q35" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="R35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="S35" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="T35" s="8" t="s">
-        <v>90</v>
+      <c r="H35" s="8">
+        <v>20</v>
+      </c>
+      <c r="I35" s="8">
+        <v>0</v>
+      </c>
+      <c r="J35" s="8">
+        <v>0</v>
+      </c>
+      <c r="K35" s="8">
+        <v>10</v>
+      </c>
+      <c r="N35" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="P35" s="8">
+        <v>20</v>
+      </c>
+      <c r="R35" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="T35" s="8">
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="B36">
+        <v>29</v>
       </c>
       <c r="D36" s="8">
         <v>50</v>
@@ -2971,112 +3036,231 @@
         <v>30</v>
       </c>
       <c r="H36" s="8">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="I36" s="8">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="J36" s="8">
-        <v>0</v>
-      </c>
-      <c r="K36" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L36" s="8">
         <v>10</v>
       </c>
       <c r="M36" s="8">
+        <v>20</v>
+      </c>
+      <c r="N36" s="8">
         <v>15</v>
       </c>
-      <c r="N36" s="8">
-        <v>7.5</v>
-      </c>
       <c r="O36" s="8">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="P36" s="8">
+        <v>30</v>
+      </c>
+      <c r="Q36" s="8">
         <v>20</v>
       </c>
-      <c r="Q36" s="8">
+      <c r="R36" s="8">
         <v>15</v>
       </c>
-      <c r="R36" s="8">
-        <v>7.5</v>
-      </c>
       <c r="S36" s="8">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="T36" s="8">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P37" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q37" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S37" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T37" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="8">
+        <v>50</v>
+      </c>
+      <c r="E38" s="8">
+        <v>60</v>
+      </c>
+      <c r="F38" s="8">
+        <v>40</v>
+      </c>
+      <c r="G38" s="8">
+        <v>30</v>
+      </c>
+      <c r="H38" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="I38" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="J38" s="8">
+        <v>0</v>
+      </c>
+      <c r="K38" s="8">
+        <v>0</v>
+      </c>
+      <c r="L38" s="8">
+        <v>10</v>
+      </c>
+      <c r="M38" s="8">
+        <v>15</v>
+      </c>
+      <c r="N38" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="O38" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="P38" s="8">
+        <v>20</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>15</v>
+      </c>
+      <c r="R38" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="S38" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="T38" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D39" s="8">
         <v>20</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E39" s="8">
         <v>60</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F39" s="8">
         <v>40</v>
       </c>
-      <c r="G37" s="8">
+      <c r="G39" s="8">
         <v>30</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H39" s="8">
         <v>7.5</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I39" s="8">
         <v>1</v>
       </c>
-      <c r="L37" s="8">
+      <c r="L39" s="8">
         <v>10</v>
       </c>
-      <c r="M37" s="8">
+      <c r="M39" s="8">
         <v>15</v>
       </c>
-      <c r="N37" s="8">
+      <c r="N39" s="8">
         <v>7.5</v>
       </c>
-      <c r="O37" s="8">
+      <c r="O39" s="8">
         <v>7.5</v>
       </c>
-      <c r="P37" s="8">
+      <c r="P39" s="8">
         <v>20</v>
       </c>
-      <c r="Q37" s="8">
+      <c r="Q39" s="8">
         <v>15</v>
       </c>
-      <c r="R37" s="8">
+      <c r="R39" s="8">
         <v>7.5</v>
       </c>
-      <c r="S37" s="8">
+      <c r="S39" s="8">
         <v>7.5</v>
       </c>
-      <c r="T37" s="8">
+      <c r="T39" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U37" xr:uid="{2A024854-562A-4BA3-B5BC-18078DDE4ADF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U37">
-      <sortCondition ref="A1:A37"/>
+  <autoFilter ref="A1:U39" xr:uid="{2A024854-562A-4BA3-B5BC-18078DDE4ADF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U39">
+      <sortCondition ref="A1:A39"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="V4" r:id="rId1" xr:uid="{F170A2A2-1E37-4B6D-9099-96A3BE49F151}"/>
+    <hyperlink ref="V20" r:id="rId2" xr:uid="{A618F85E-D5C5-4A05-9872-B508E2E25A31}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>